<commit_message>
Add test case to fancy-test spreadsheet
This reproduces a blank-column issue seen in issue #35
</commit_message>
<xml_diff>
--- a/data/fancy-test.xlsx
+++ b/data/fancy-test.xlsx
@@ -1,32 +1,42 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joe\Documents\Demo Data\Demo data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joequigley/code/jupyterlab-spreadsheet/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{6C5C5763-8876-4A5F-B85A-25131C078D6C}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{854BD643-BE05-7F46-BA6D-348DD58C8342}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13680" windowHeight="7425" activeTab="1" xr2:uid="{4B8492F7-FD0E-490D-802A-218599838A94}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="2" xr2:uid="{4B8492F7-FD0E-490D-802A-218599838A94}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
   <si>
     <t>TEst</t>
   </si>
@@ -104,6 +114,15 @@
   </si>
   <si>
     <t>avg</t>
+  </si>
+  <si>
+    <t>&lt; that is column D</t>
+  </si>
+  <si>
+    <t>&lt; it should be ~2x wide</t>
+  </si>
+  <si>
+    <t>&lt; as column E</t>
   </si>
 </sst>
 </file>
@@ -163,9 +182,6 @@
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" textRotation="45"/>
@@ -175,6 +191,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment textRotation="135"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -496,67 +515,67 @@
       <selection activeCell="A6" sqref="A6:B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A2" s="1"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="5"/>
       <c r="B2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1" t="s">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="5"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="5"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-    </row>
-    <row r="7" spans="1:4" ht="15.4" x14ac:dyDescent="0.6">
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="5"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="1"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1" t="s">
+      <c r="C7" s="5"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="5"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="5"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>1</v>
       </c>
@@ -588,50 +607,62 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73DC9FA1-8290-4166-B823-47819E2203EB}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="16.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="45" x14ac:dyDescent="0.45">
-      <c r="B2" s="5" t="s">
+    <row r="2" spans="1:5" ht="46" x14ac:dyDescent="0.2">
+      <c r="B2" s="4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="E3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C4">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="E4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C5">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="43.5" x14ac:dyDescent="0.45">
-      <c r="B6" s="4" t="s">
+    <row r="6" spans="1:5" ht="47" x14ac:dyDescent="0.2">
+      <c r="B6" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="2">
         <f>SUM(C3:C5)</f>
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="B7" s="2" t="s">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B7" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C7">
@@ -643,4 +674,34 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04E81871-1DB9-4440-BA05-B0D4FFA7E2D7}">
+  <dimension ref="B1:B3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B3">
+        <v>123</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update test sheet with new test cases
</commit_message>
<xml_diff>
--- a/data/fancy-test.xlsx
+++ b/data/fancy-test.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joequigley/code/jupyterlab-spreadsheet/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{854BD643-BE05-7F46-BA6D-348DD58C8342}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD3E59D7-49BC-8D4F-A028-6805646454BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="2" xr2:uid="{4B8492F7-FD0E-490D-802A-218599838A94}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="empty first col and row" sheetId="3" r:id="rId3"/>
+    <sheet name="empty sheet!" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -678,30 +679,42 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04E81871-1DB9-4440-BA05-B0D4FFA7E2D7}">
-  <dimension ref="B1:B3"/>
+  <dimension ref="B2:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-    </row>
     <row r="2" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B3">
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B4">
         <v>123</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFD379A8-5133-5E4C-AD29-CF10DBF10B5B}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>